<commit_message>
Kingdom Buy Api 로직 작성 / PlacedKingdomItem 모델 추가
</commit_message>
<xml_diff>
--- a/Data/Excel/Model/User/PlacedKingdomItem.xlsx
+++ b/Data/Excel/Model/User/PlacedKingdomItem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitWorks\GameServerStudyAspNet\Data\Excel\Model\User\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FC9DCE-F951-40E1-97E4-DC0323539E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7698FF54-3480-4455-BA96-03A1042592EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -106,23 +106,15 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>fk</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>c_index</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>#PlayerId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>#Id</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Packet</t>
+    <t>Id</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlayerId</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1060,7 +1052,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E12"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
@@ -1092,13 +1084,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
@@ -1125,12 +1114,6 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -1139,11 +1122,8 @@
       <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1153,9 +1133,6 @@
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -1164,9 +1141,6 @@
       <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -1175,9 +1149,6 @@
       <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -1186,9 +1157,6 @@
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="E9" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -1197,9 +1165,6 @@
       <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="E10" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -1208,9 +1173,6 @@
       <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="E11" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -1218,9 +1180,6 @@
       </c>
       <c r="B12" t="s">
         <v>5</v>
-      </c>
-      <c r="E12" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>